<commit_message>
HS Component for Authority Management
</commit_message>
<xml_diff>
--- a/vertx-pin/zero-wf/src/main/resources/plugin/wf/oob/data/authority.flow.xlsx
+++ b/vertx-pin/zero-wf/src/main/resources/plugin/wf/oob/data/authority.flow.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/var/folders/lm/r14tlhyj7fncnytfwf3v8dc00000gn/T/tmp-37191-xqnJf3Po2pZB/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/var/folders/lm/r14tlhyj7fncnytfwf3v8dc00000gn/T/tmp-22948-k6SwkU82ogL4/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C73F0672-59C7-D542-A4CB-03F0BB8F02EA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2E91774D-BA33-8542-B87C-DC3E17EC1183}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="38500" yWindow="3660" windowWidth="38400" windowHeight="20340" xr2:uid="{BC32819D-176D-6D4B-8CEE-9D375DE1CDB6}"/>
+    <workbookView xWindow="58380" yWindow="-1520" windowWidth="38400" windowHeight="20340" xr2:uid="{BC32819D-176D-6D4B-8CEE-9D375DE1CDB6}"/>
   </bookViews>
   <sheets>
     <sheet name="DATA-RULE" sheetId="2" r:id="rId1"/>
@@ -309,10 +309,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>io.vertx.tp.rbac.ruler.HSDimDao</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>JSON:authority/auth.flow/dm.condition.json</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -360,6 +356,10 @@
   </si>
   <si>
     <t>列表权限</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>io.vertx.tp.rbac.ruler.HSDimArea</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -991,8 +991,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F4D6C9C3-8DFE-A442-A082-10767386D931}">
   <dimension ref="A3:Q8"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I6" sqref="I6"/>
+    <sheetView tabSelected="1" topLeftCell="K1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="P6" sqref="P6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="18"/>
@@ -1047,7 +1047,7 @@
         <v>17</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C4" s="4" t="s">
         <v>18</v>
@@ -1100,7 +1100,7 @@
         <v>0</v>
       </c>
       <c r="B5" s="6" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C5" s="6" t="s">
         <v>5</v>
@@ -1157,7 +1157,7 @@
         <v>64</v>
       </c>
       <c r="D6" s="9" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="E6" s="11" t="s">
         <v>68</v>
@@ -1173,7 +1173,7 @@
       </c>
       <c r="I6" s="10"/>
       <c r="J6" s="10" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="K6" s="9" t="s">
         <v>66</v>
@@ -1185,34 +1185,34 @@
         <v>30</v>
       </c>
       <c r="N6" s="10" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="O6" s="9" t="s">
         <v>67</v>
       </c>
       <c r="P6" s="9" t="s">
-        <v>69</v>
+        <v>82</v>
       </c>
       <c r="Q6" s="9" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="7" spans="1:17">
       <c r="A7" s="9" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B7" s="9" t="str">
         <f>A$6</f>
         <v>9455c4f4-dfcc-4cb4-a31e-6dcf5772e6ed</v>
       </c>
       <c r="C7" s="9" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="D7" s="9" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="E7" s="11" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="F7" s="11" t="s">
         <v>41</v>
@@ -1235,20 +1235,20 @@
     </row>
     <row r="8" spans="1:17">
       <c r="A8" s="9" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B8" s="9" t="str">
         <f>A$6</f>
         <v>9455c4f4-dfcc-4cb4-a31e-6dcf5772e6ed</v>
       </c>
       <c r="C8" s="9" t="s">
+        <v>75</v>
+      </c>
+      <c r="D8" s="9" t="s">
         <v>76</v>
       </c>
-      <c r="D8" s="9" t="s">
-        <v>77</v>
-      </c>
       <c r="E8" s="11" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="F8" s="11" t="s">
         <v>41</v>

</xml_diff>